<commit_message>
Add OA vs CH
</commit_message>
<xml_diff>
--- a/BenchmarkingFramework/BenchmarkingFramework/Database/Database BEST.xlsx
+++ b/BenchmarkingFramework/BenchmarkingFramework/Database/Database BEST.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Graphs" sheetId="12" r:id="rId2"/>
     <sheet name="Table" sheetId="11" r:id="rId3"/>
     <sheet name="Pivot" sheetId="10" r:id="rId4"/>
-    <sheet name="AVL vs OA, CH lookup" sheetId="18" r:id="rId5"/>
+    <sheet name="AVL vs OA vs CH lookup" sheetId="18" r:id="rId5"/>
     <sheet name="Database" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2166" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2272" uniqueCount="49">
   <si>
     <t>id</t>
   </si>
@@ -140,9 +140,6 @@
     <t>AVL</t>
   </si>
   <si>
-    <t>Open Add</t>
-  </si>
-  <si>
     <t>lookup</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>CH</t>
+  </si>
+  <si>
+    <t>OA</t>
   </si>
 </sst>
 </file>
@@ -1339,6 +1339,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1837,6 +1838,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4094,6 +4096,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4592,6 +4595,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4703,6 +4707,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5201,6 +5206,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5312,6 +5318,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5810,6 +5817,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5920,6 +5928,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6418,6 +6427,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -23447,8 +23457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24806,41 +24816,49 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I112"/>
+  <dimension ref="A1:N112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
         <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="H1" t="s">
         <v>36</v>
       </c>
       <c r="I1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
@@ -24848,9 +24866,12 @@
       <c r="G2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
         <v>23</v>
@@ -24865,8 +24886,15 @@
       <c r="I4" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L4" s="7"/>
+      <c r="M4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>25</v>
       </c>
@@ -24885,8 +24913,17 @@
       <c r="I5" s="5">
         <v>3.3950000000000048E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="5">
+        <v>3.9125000000000071E-3</v>
+      </c>
+      <c r="N5" s="5">
+        <v>3.3950000000000048E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>26</v>
       </c>
@@ -24905,8 +24942,17 @@
       <c r="I6" s="5">
         <v>3.2878817948718016E-4</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="5">
+        <v>2.7627548076923121E-4</v>
+      </c>
+      <c r="N6" s="5">
+        <v>3.2878817948718016E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>27</v>
       </c>
@@ -24925,8 +24971,17 @@
       <c r="I7" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="5">
+        <v>40</v>
+      </c>
+      <c r="N7" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -24941,8 +24996,15 @@
         <v>0</v>
       </c>
       <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" s="5">
+        <v>0</v>
+      </c>
+      <c r="N8" s="5"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>29</v>
       </c>
@@ -24957,8 +25019,15 @@
         <v>63</v>
       </c>
       <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9" s="5">
+        <v>77</v>
+      </c>
+      <c r="N9" s="5"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>30</v>
       </c>
@@ -24973,8 +25042,15 @@
         <v>0.45317512244662933</v>
       </c>
       <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" s="5">
+        <v>0.1330576395169755</v>
+      </c>
+      <c r="N10" s="5"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>31</v>
       </c>
@@ -24989,8 +25065,15 @@
         <v>0.32598982622532641</v>
       </c>
       <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M11" s="5">
+        <v>0.44724745843681307</v>
+      </c>
+      <c r="N11" s="5"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>32</v>
       </c>
@@ -25005,8 +25088,15 @@
         <v>1.6694022217068125</v>
       </c>
       <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M12" s="5">
+        <v>1.6648845372582084</v>
+      </c>
+      <c r="N12" s="5"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>33</v>
       </c>
@@ -25021,8 +25111,15 @@
         <v>0.65197965245065281</v>
       </c>
       <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M13" s="5">
+        <v>0.89449491687362614</v>
+      </c>
+      <c r="N13" s="5"/>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>34</v>
       </c>
@@ -25037,10 +25134,17 @@
         <v>1.9983405425207412</v>
       </c>
       <c r="I14" s="6"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M14" s="6">
+        <v>1.9912543953883848</v>
+      </c>
+      <c r="N14" s="6"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
         <v>35</v>
@@ -25048,9 +25152,12 @@
       <c r="G16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
       <c r="C18" s="7" t="s">
         <v>23</v>
@@ -25065,8 +25172,15 @@
       <c r="I18" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L18" s="7"/>
+      <c r="M18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>25</v>
       </c>
@@ -25085,8 +25199,17 @@
       <c r="I19" s="5">
         <v>6.9424999999999999E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M19" s="5">
+        <v>1.0437499999999994E-2</v>
+      </c>
+      <c r="N19" s="5">
+        <v>6.9424999999999999E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>26</v>
       </c>
@@ -25105,8 +25228,17 @@
       <c r="I20" s="5">
         <v>1.4491532692307695E-4</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M20" s="5">
+        <v>3.2598397435897424E-6</v>
+      </c>
+      <c r="N20" s="5">
+        <v>1.4491532692307695E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>27</v>
       </c>
@@ -25125,8 +25257,17 @@
       <c r="I21" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L21" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M21" s="5">
+        <v>40</v>
+      </c>
+      <c r="N21" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>28</v>
       </c>
@@ -25141,8 +25282,15 @@
         <v>0</v>
       </c>
       <c r="I22" s="5"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M22" s="5">
+        <v>0</v>
+      </c>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>29</v>
       </c>
@@ -25157,8 +25305,15 @@
         <v>44</v>
       </c>
       <c r="I23" s="5"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M23" s="5">
+        <v>41</v>
+      </c>
+      <c r="N23" s="5"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>30</v>
       </c>
@@ -25173,8 +25328,15 @@
         <v>2.9754682282283031</v>
       </c>
       <c r="I24" s="5"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M24" s="5">
+        <v>1.8158896928436168</v>
+      </c>
+      <c r="N24" s="5"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>31</v>
       </c>
@@ -25189,8 +25351,15 @@
         <v>2.3689066307704221E-3</v>
       </c>
       <c r="I25" s="5"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M25" s="5">
+        <v>3.8352461826049782E-2</v>
+      </c>
+      <c r="N25" s="5"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>32</v>
       </c>
@@ -25205,8 +25374,15 @@
         <v>1.680229976572116</v>
       </c>
       <c r="I26" s="5"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L26" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M26" s="5">
+        <v>1.6828780021327077</v>
+      </c>
+      <c r="N26" s="5"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>33</v>
       </c>
@@ -25221,8 +25397,15 @@
         <v>4.7378132615408441E-3</v>
       </c>
       <c r="I27" s="5"/>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L27" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M27" s="5">
+        <v>7.6704923652099563E-2</v>
+      </c>
+      <c r="N27" s="5"/>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
         <v>34</v>
       </c>
@@ -25237,10 +25420,17 @@
         <v>2.0153675744437649</v>
       </c>
       <c r="I28" s="6"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L28" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M28" s="6">
+        <v>2.0195409704413767</v>
+      </c>
+      <c r="N28" s="6"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
         <v>35</v>
@@ -25248,9 +25438,12 @@
       <c r="G30" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
         <v>23</v>
@@ -25265,8 +25458,15 @@
       <c r="I32" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L32" s="7"/>
+      <c r="M32" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N32" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>25</v>
       </c>
@@ -25285,8 +25485,17 @@
       <c r="I33" s="5">
         <v>2.4032499999999998E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M33" s="5">
+        <v>5.74975E-2</v>
+      </c>
+      <c r="N33" s="5">
+        <v>2.4032499999999998E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>26</v>
       </c>
@@ -25305,8 +25514,17 @@
       <c r="I34" s="5">
         <v>4.4243275641025754E-5</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L34" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M34" s="5">
+        <v>7.3141275641025883E-5</v>
+      </c>
+      <c r="N34" s="5">
+        <v>4.4243275641025754E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>27</v>
       </c>
@@ -25325,8 +25543,17 @@
       <c r="I35" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L35" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M35" s="5">
+        <v>40</v>
+      </c>
+      <c r="N35" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>28</v>
       </c>
@@ -25341,8 +25568,15 @@
         <v>0</v>
       </c>
       <c r="I36" s="5"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L36" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M36" s="5">
+        <v>0</v>
+      </c>
+      <c r="N36" s="5"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>29</v>
       </c>
@@ -25357,8 +25591,15 @@
         <v>69</v>
       </c>
       <c r="I37" s="5"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L37" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M37" s="5">
+        <v>74</v>
+      </c>
+      <c r="N37" s="5"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>30</v>
       </c>
@@ -25373,8 +25614,15 @@
         <v>27.207984297909622</v>
       </c>
       <c r="I38" s="5"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L38" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M38" s="5">
+        <v>19.535087144973311</v>
+      </c>
+      <c r="N38" s="5"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>31</v>
       </c>
@@ -25389,8 +25637,15 @@
         <v>6.4518387841331758E-39</v>
       </c>
       <c r="I39" s="5"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L39" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M39" s="5">
+        <v>3.1296475174827372E-31</v>
+      </c>
+      <c r="N39" s="5"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>32</v>
       </c>
@@ -25405,8 +25660,15 @@
         <v>1.6672385486685533</v>
       </c>
       <c r="I40" s="5"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L40" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M40" s="5">
+        <v>1.6657068927340244</v>
+      </c>
+      <c r="N40" s="5"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>33</v>
       </c>
@@ -25421,8 +25683,15 @@
         <v>1.2903677568266352E-38</v>
       </c>
       <c r="I41" s="5"/>
-    </row>
-    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L41" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M41" s="5">
+        <v>6.2592950349654744E-31</v>
+      </c>
+      <c r="N41" s="5"/>
+    </row>
+    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="6" t="s">
         <v>34</v>
       </c>
@@ -25437,10 +25706,17 @@
         <v>1.9949454151072357</v>
       </c>
       <c r="I42" s="6"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L42" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M42" s="6">
+        <v>1.992543495180934</v>
+      </c>
+      <c r="N42" s="6"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
         <v>35</v>
@@ -25448,9 +25724,12 @@
       <c r="G44" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B46" s="7"/>
       <c r="C46" s="7" t="s">
         <v>23</v>
@@ -25465,8 +25744,15 @@
       <c r="I46" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L46" s="7"/>
+      <c r="M46" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N46" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>25</v>
       </c>
@@ -25485,8 +25771,17 @@
       <c r="I47" s="5">
         <v>4.6019999999999991E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L47" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M47" s="5">
+        <v>0.1169625</v>
+      </c>
+      <c r="N47" s="5">
+        <v>4.6019999999999991E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
         <v>26</v>
       </c>
@@ -25505,8 +25800,17 @@
       <c r="I48" s="5">
         <v>6.0153948717949041E-5</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L48" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M48" s="5">
+        <v>1.1594444551282096E-3</v>
+      </c>
+      <c r="N48" s="5">
+        <v>6.0153948717949041E-5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
         <v>27</v>
       </c>
@@ -25525,8 +25829,17 @@
       <c r="I49" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L49" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M49" s="5">
+        <v>40</v>
+      </c>
+      <c r="N49" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
         <v>28</v>
       </c>
@@ -25541,8 +25854,15 @@
         <v>0</v>
       </c>
       <c r="I50" s="5"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L50" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M50" s="5">
+        <v>0</v>
+      </c>
+      <c r="N50" s="5"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
         <v>29</v>
       </c>
@@ -25557,8 +25877,15 @@
         <v>46</v>
       </c>
       <c r="I51" s="5"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L51" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M51" s="5">
+        <v>43</v>
+      </c>
+      <c r="N51" s="5"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
         <v>30</v>
       </c>
@@ -25573,8 +25900,15 @@
         <v>27.563034075767256</v>
       </c>
       <c r="I52" s="5"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L52" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M52" s="5">
+        <v>12.847779099106956</v>
+      </c>
+      <c r="N52" s="5"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
         <v>31</v>
       </c>
@@ -25589,8 +25923,15 @@
         <v>1.5155645252272997E-30</v>
       </c>
       <c r="I53" s="5"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L53" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M53" s="5">
+        <v>1.2814922556804546E-16</v>
+      </c>
+      <c r="N53" s="5"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
         <v>32</v>
       </c>
@@ -25605,8 +25946,15 @@
         <v>1.678660413556865</v>
       </c>
       <c r="I54" s="5"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L54" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M54" s="5">
+        <v>1.6810707032025196</v>
+      </c>
+      <c r="N54" s="5"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
         <v>33</v>
       </c>
@@ -25621,8 +25969,15 @@
         <v>3.0311290504545994E-30</v>
       </c>
       <c r="I55" s="5"/>
-    </row>
-    <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L55" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M55" s="5">
+        <v>2.5629845113609093E-16</v>
+      </c>
+      <c r="N55" s="5"/>
+    </row>
+    <row r="56" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="6" t="s">
         <v>34</v>
       </c>
@@ -25637,10 +25992,17 @@
         <v>2.0128955989194299</v>
       </c>
       <c r="I56" s="6"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L56" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M56" s="6">
+        <v>2.0166921992278248</v>
+      </c>
+      <c r="N56" s="6"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B58" t="s">
         <v>35</v>
@@ -25648,9 +26010,12 @@
       <c r="G58" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L58" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B60" s="7"/>
       <c r="C60" s="7" t="s">
         <v>23</v>
@@ -25665,8 +26030,15 @@
       <c r="I60" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L60" s="7"/>
+      <c r="M60" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N60" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B61" s="5" t="s">
         <v>25</v>
       </c>
@@ -25685,8 +26057,17 @@
       <c r="I61" s="5">
         <v>4.4610000000000004E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L61" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M61" s="5">
+        <v>0.12619250000000001</v>
+      </c>
+      <c r="N61" s="5">
+        <v>4.4610000000000004E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B62" s="5" t="s">
         <v>26</v>
       </c>
@@ -25705,8 +26086,17 @@
       <c r="I62" s="5">
         <v>8.1451692307691064E-5</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L62" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M62" s="5">
+        <v>7.8894224999999547E-4</v>
+      </c>
+      <c r="N62" s="5">
+        <v>8.1451692307691064E-5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B63" s="5" t="s">
         <v>27</v>
       </c>
@@ -25725,8 +26115,17 @@
       <c r="I63" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L63" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M63" s="5">
+        <v>40</v>
+      </c>
+      <c r="N63" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B64" s="5" t="s">
         <v>28</v>
       </c>
@@ -25741,8 +26140,15 @@
         <v>0</v>
       </c>
       <c r="I64" s="5"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L64" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M64" s="5">
+        <v>0</v>
+      </c>
+      <c r="N64" s="5"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B65" s="5" t="s">
         <v>29</v>
       </c>
@@ -25757,8 +26163,15 @@
         <v>48</v>
       </c>
       <c r="I65" s="5"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L65" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M65" s="5">
+        <v>47</v>
+      </c>
+      <c r="N65" s="5"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B66" s="5" t="s">
         <v>30</v>
       </c>
@@ -25773,8 +26186,15 @@
         <v>39.413162062426572</v>
       </c>
       <c r="I66" s="5"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L66" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M66" s="5">
+        <v>17.48916501245558</v>
+      </c>
+      <c r="N66" s="5"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B67" s="5" t="s">
         <v>31</v>
       </c>
@@ -25789,8 +26209,15 @@
         <v>1.607604225426845E-38</v>
       </c>
       <c r="I67" s="5"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L67" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M67" s="5">
+        <v>1.6503106779652564E-22</v>
+      </c>
+      <c r="N67" s="5"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B68" s="5" t="s">
         <v>32</v>
       </c>
@@ -25805,8 +26232,15 @@
         <v>1.6772241961243386</v>
       </c>
       <c r="I68" s="5"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L68" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M68" s="5">
+        <v>1.6779267216418625</v>
+      </c>
+      <c r="N68" s="5"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B69" s="5" t="s">
         <v>33</v>
       </c>
@@ -25821,8 +26255,15 @@
         <v>3.2152084508536901E-38</v>
       </c>
       <c r="I69" s="5"/>
-    </row>
-    <row r="70" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L69" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M69" s="5">
+        <v>3.3006213559305127E-22</v>
+      </c>
+      <c r="N69" s="5"/>
+    </row>
+    <row r="70" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="6" t="s">
         <v>34</v>
       </c>
@@ -25837,10 +26278,17 @@
         <v>2.0106347576242314</v>
       </c>
       <c r="I70" s="6"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L70" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M70" s="6">
+        <v>2.0117405137297668</v>
+      </c>
+      <c r="N70" s="6"/>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B72" t="s">
         <v>35</v>
@@ -25848,9 +26296,12 @@
       <c r="G72" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L72" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B74" s="7"/>
       <c r="C74" s="7" t="s">
         <v>23</v>
@@ -25865,8 +26316,15 @@
       <c r="I74" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L74" s="7"/>
+      <c r="M74" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N74" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B75" s="5" t="s">
         <v>25</v>
       </c>
@@ -25885,8 +26343,17 @@
       <c r="I75" s="5">
         <v>4.6012499999999998E-2</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L75" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M75" s="5">
+        <v>0.1396075</v>
+      </c>
+      <c r="N75" s="5">
+        <v>4.6012499999999998E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B76" s="5" t="s">
         <v>26</v>
       </c>
@@ -25905,8 +26372,17 @@
       <c r="I76" s="5">
         <v>9.4919583333334209E-5</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L76" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M76" s="5">
+        <v>1.1356089166666701E-3</v>
+      </c>
+      <c r="N76" s="5">
+        <v>9.4919583333334209E-5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B77" s="5" t="s">
         <v>27</v>
       </c>
@@ -25925,8 +26401,17 @@
       <c r="I77" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L77" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M77" s="5">
+        <v>40</v>
+      </c>
+      <c r="N77" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B78" s="5" t="s">
         <v>28</v>
       </c>
@@ -25941,8 +26426,15 @@
         <v>0</v>
       </c>
       <c r="I78" s="5"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L78" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M78" s="5">
+        <v>0</v>
+      </c>
+      <c r="N78" s="5"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B79" s="5" t="s">
         <v>29</v>
       </c>
@@ -25957,8 +26449,15 @@
         <v>40</v>
       </c>
       <c r="I79" s="5"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L79" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M79" s="5">
+        <v>45</v>
+      </c>
+      <c r="N79" s="5"/>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B80" s="5" t="s">
         <v>30</v>
       </c>
@@ -25973,8 +26472,15 @@
         <v>17.41979151836675</v>
       </c>
       <c r="I80" s="5"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L80" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M80" s="5">
+        <v>16.874728957815897</v>
+      </c>
+      <c r="N80" s="5"/>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B81" s="5" t="s">
         <v>31</v>
       </c>
@@ -25989,8 +26495,15 @@
         <v>1.4016915455984687E-20</v>
       </c>
       <c r="I81" s="5"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L81" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M81" s="5">
+        <v>2.1889402022347875E-21</v>
+      </c>
+      <c r="N81" s="5"/>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B82" s="5" t="s">
         <v>32</v>
       </c>
@@ -26005,8 +26518,15 @@
         <v>1.6838510133356521</v>
       </c>
       <c r="I82" s="5"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L82" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M82" s="5">
+        <v>1.6794273926523535</v>
+      </c>
+      <c r="N82" s="5"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B83" s="5" t="s">
         <v>33</v>
       </c>
@@ -26021,8 +26541,15 @@
         <v>2.8033830911969374E-20</v>
       </c>
       <c r="I83" s="5"/>
-    </row>
-    <row r="84" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L83" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M83" s="5">
+        <v>4.377880404469575E-21</v>
+      </c>
+      <c r="N83" s="5"/>
+    </row>
+    <row r="84" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B84" s="6" t="s">
         <v>34</v>
       </c>
@@ -26037,10 +26564,17 @@
         <v>2.0210753903062737</v>
       </c>
       <c r="I84" s="6"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L84" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M84" s="6">
+        <v>2.0141033888808457</v>
+      </c>
+      <c r="N84" s="6"/>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B86" t="s">
         <v>35</v>
@@ -26048,9 +26582,12 @@
       <c r="G86" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L86" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B88" s="7"/>
       <c r="C88" s="7" t="s">
         <v>23</v>
@@ -26065,8 +26602,15 @@
       <c r="I88" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L88" s="7"/>
+      <c r="M88" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N88" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B89" s="5" t="s">
         <v>25</v>
       </c>
@@ -26085,8 +26629,17 @@
       <c r="I89" s="5">
         <v>5.5717499999999996E-2</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L89" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M89" s="5">
+        <v>0.105545</v>
+      </c>
+      <c r="N89" s="5">
+        <v>5.5717499999999996E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B90" s="5" t="s">
         <v>26</v>
       </c>
@@ -26105,8 +26658,17 @@
       <c r="I90" s="5">
         <v>6.0710148076923126E-4</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L90" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M90" s="5">
+        <v>9.3670356410256554E-4</v>
+      </c>
+      <c r="N90" s="5">
+        <v>6.0710148076923126E-4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B91" s="5" t="s">
         <v>27</v>
       </c>
@@ -26125,8 +26687,17 @@
       <c r="I91" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L91" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M91" s="5">
+        <v>40</v>
+      </c>
+      <c r="N91" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B92" s="5" t="s">
         <v>28</v>
       </c>
@@ -26141,8 +26712,15 @@
         <v>0</v>
       </c>
       <c r="I92" s="5"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L92" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M92" s="5">
+        <v>0</v>
+      </c>
+      <c r="N92" s="5"/>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B93" s="5" t="s">
         <v>29</v>
       </c>
@@ -26157,8 +26735,15 @@
         <v>45</v>
       </c>
       <c r="I93" s="5"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L93" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M93" s="5">
+        <v>75</v>
+      </c>
+      <c r="N93" s="5"/>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B94" s="5" t="s">
         <v>30</v>
       </c>
@@ -26173,8 +26758,15 @@
         <v>18.647048497305285</v>
       </c>
       <c r="I94" s="5"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L94" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M94" s="5">
+        <v>8.0205262693308512</v>
+      </c>
+      <c r="N94" s="5"/>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B95" s="5" t="s">
         <v>31</v>
       </c>
@@ -26189,8 +26781,15 @@
         <v>4.2435825024626314E-23</v>
       </c>
       <c r="I95" s="5"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L95" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M95" s="5">
+        <v>5.4532873128070489E-12</v>
+      </c>
+      <c r="N95" s="5"/>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B96" s="5" t="s">
         <v>32</v>
       </c>
@@ -26205,8 +26804,15 @@
         <v>1.6794273926523535</v>
       </c>
       <c r="I96" s="5"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L96" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M96" s="5">
+        <v>1.6654253733225626</v>
+      </c>
+      <c r="N96" s="5"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B97" s="5" t="s">
         <v>33</v>
       </c>
@@ -26221,8 +26827,15 @@
         <v>8.4871650049252629E-23</v>
       </c>
       <c r="I97" s="5"/>
-    </row>
-    <row r="98" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L97" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M97" s="5">
+        <v>1.0906574625614098E-11</v>
+      </c>
+      <c r="N97" s="5"/>
+    </row>
+    <row r="98" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B98" s="6" t="s">
         <v>34</v>
       </c>
@@ -26237,10 +26850,17 @@
         <v>2.0141033888808457</v>
       </c>
       <c r="I98" s="6"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L98" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M98" s="6">
+        <v>1.9921021540022406</v>
+      </c>
+      <c r="N98" s="6"/>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B100" t="s">
         <v>35</v>
@@ -26248,9 +26868,12 @@
       <c r="G100" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L100" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B102" s="7"/>
       <c r="C102" s="7" t="s">
         <v>23</v>
@@ -26265,8 +26888,15 @@
       <c r="I102" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L102" s="7"/>
+      <c r="M102" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N102" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B103" s="5" t="s">
         <v>25</v>
       </c>
@@ -26285,8 +26915,17 @@
       <c r="I103" s="5">
         <v>5.3767500000000024E-2</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L103" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M103" s="5">
+        <v>0.11431794871794868</v>
+      </c>
+      <c r="N103" s="5">
+        <v>5.3767500000000024E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B104" s="5" t="s">
         <v>26</v>
       </c>
@@ -26305,8 +26944,17 @@
       <c r="I104" s="5">
         <v>1.9398327564102368E-4</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L104" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M104" s="5">
+        <v>4.2111309041836505E-4</v>
+      </c>
+      <c r="N104" s="5">
+        <v>1.9398327564102368E-4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B105" s="5" t="s">
         <v>27</v>
       </c>
@@ -26325,8 +26973,17 @@
       <c r="I105" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L105" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M105" s="5">
+        <v>39</v>
+      </c>
+      <c r="N105" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B106" s="5" t="s">
         <v>28</v>
       </c>
@@ -26341,8 +26998,15 @@
         <v>0</v>
       </c>
       <c r="I106" s="5"/>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L106" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M106" s="5">
+        <v>0</v>
+      </c>
+      <c r="N106" s="5"/>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B107" s="5" t="s">
         <v>29</v>
       </c>
@@ -26357,8 +27021,15 @@
         <v>41</v>
       </c>
       <c r="I107" s="5"/>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L107" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M107" s="5">
+        <v>67</v>
+      </c>
+      <c r="N107" s="5"/>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B108" s="5" t="s">
         <v>30</v>
       </c>
@@ -26373,8 +27044,15 @@
         <v>21.053580633626751</v>
       </c>
       <c r="I108" s="5"/>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L108" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M108" s="5">
+        <v>15.307240992948863</v>
+      </c>
+      <c r="N108" s="5"/>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B109" s="5" t="s">
         <v>31</v>
       </c>
@@ -26389,8 +27067,15 @@
         <v>6.7333755055166803E-24</v>
       </c>
       <c r="I109" s="5"/>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L109" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M109" s="5">
+        <v>7.3376117249955237E-24</v>
+      </c>
+      <c r="N109" s="5"/>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B110" s="5" t="s">
         <v>32</v>
       </c>
@@ -26405,8 +27090,15 @@
         <v>1.6828780021327077</v>
       </c>
       <c r="I110" s="5"/>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L110" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M110" s="5">
+        <v>1.6679161141074239</v>
+      </c>
+      <c r="N110" s="5"/>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B111" s="5" t="s">
         <v>33</v>
       </c>
@@ -26421,8 +27113,15 @@
         <v>1.3466751011033361E-23</v>
       </c>
       <c r="I111" s="5"/>
-    </row>
-    <row r="112" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L111" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M111" s="5">
+        <v>1.4675223449991047E-23</v>
+      </c>
+      <c r="N111" s="5"/>
+    </row>
+    <row r="112" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B112" s="6" t="s">
         <v>34</v>
       </c>
@@ -26437,6 +27136,13 @@
         <v>2.0195409704413767</v>
       </c>
       <c r="I112" s="6"/>
+      <c r="L112" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M112" s="6">
+        <v>1.9960083540252964</v>
+      </c>
+      <c r="N112" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26449,8 +27155,8 @@
   <dimension ref="A1:K961"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A938" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M899" sqref="M899"/>
+      <pane ySplit="1" topLeftCell="A929" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H717" sqref="H717"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45048,7 +45754,7 @@
         <v>2097184</v>
       </c>
       <c r="K641" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="642" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>